<commit_message>
Modify createscript to generate tests with 200 and 500 scenarios Modify the policy Re-solve to use RQMC change the average of slowmoving to 1 Modify the transform of Lumpy Create a scrpt generation method for the Quebec grid
</commit_message>
<xml_diff>
--- a/Instances/01_SlowMoving.xlsx
+++ b/Instances/01_SlowMoving.xlsx
@@ -840,13 +840,13 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="D2" t="n">
         <v>0.026</v>
       </c>
       <c r="E2" t="n">
-        <v>2.36</v>
+        <v>0.41</v>
       </c>
       <c r="F2" t="n">
         <v>0.26</v>
@@ -869,13 +869,13 @@
         <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="D3" t="n">
         <v>0.0248</v>
       </c>
       <c r="E3" t="n">
-        <v>2.1</v>
+        <v>0.47</v>
       </c>
       <c r="F3" t="n">
         <v>0.248</v>
@@ -898,13 +898,13 @@
         <v>1</v>
       </c>
       <c r="C4" t="n">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="D4" t="n">
         <v>0.0048</v>
       </c>
       <c r="E4" t="n">
-        <v>3.45</v>
+        <v>0.86</v>
       </c>
       <c r="F4" t="n">
         <v>0.048</v>
@@ -927,13 +927,13 @@
         <v>1</v>
       </c>
       <c r="C5" t="n">
-        <v>35</v>
+        <v>6</v>
       </c>
       <c r="D5" t="n">
         <v>0.002</v>
       </c>
       <c r="E5" t="n">
-        <v>3.37</v>
+        <v>0.72</v>
       </c>
       <c r="F5" t="n">
         <v>0.02</v>
@@ -956,13 +956,13 @@
         <v>1</v>
       </c>
       <c r="C6" t="n">
-        <v>37</v>
+        <v>4</v>
       </c>
       <c r="D6" t="n">
         <v>0.0036</v>
       </c>
       <c r="E6" t="n">
-        <v>3.81</v>
+        <v>0.91</v>
       </c>
       <c r="F6" t="n">
         <v>0.036</v>
@@ -985,19 +985,19 @@
         <v>1</v>
       </c>
       <c r="C7" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D7" t="n">
         <v>0.026</v>
       </c>
       <c r="E7" t="n">
-        <v>1.07</v>
+        <v>0.21</v>
       </c>
       <c r="F7" t="n">
         <v>0.26</v>
       </c>
       <c r="G7" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H7" t="n">
         <v>36.62</v>
@@ -1014,19 +1014,19 @@
         <v>1</v>
       </c>
       <c r="C8" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D8" t="n">
         <v>0.0508</v>
       </c>
       <c r="E8" t="n">
-        <v>0.82</v>
+        <v>0.22</v>
       </c>
       <c r="F8" t="n">
         <v>0.508</v>
       </c>
       <c r="G8" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H8" t="n">
         <v>1</v>
@@ -1043,19 +1043,19 @@
         <v>1</v>
       </c>
       <c r="C9" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D9" t="n">
         <v>0.0248</v>
       </c>
       <c r="E9" t="n">
-        <v>1.18</v>
+        <v>0.2</v>
       </c>
       <c r="F9" t="n">
         <v>0.248</v>
       </c>
       <c r="G9" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H9" t="n">
         <v>2</v>
@@ -1093,7 +1093,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>36</v>
+        <v>14.4</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1101,7 +1101,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>18</v>
+        <v>3.6</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1109,7 +1109,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>180</v>
+        <v>21.6</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1117,7 +1117,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>36</v>
+        <v>28.8</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1125,7 +1125,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>144</v>
+        <v>21.6</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1141,7 +1141,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>18</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1149,7 +1149,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>45</v>
+        <v>7.2</v>
       </c>
     </row>
   </sheetData>
@@ -1202,7 +1202,7 @@
         <v>9</v>
       </c>
       <c r="B2" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
@@ -1266,7 +1266,7 @@
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
@@ -1298,7 +1298,7 @@
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F5" t="n">
         <v>0</v>
@@ -1330,7 +1330,7 @@
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G6" t="n">
         <v>0</v>
@@ -1362,7 +1362,7 @@
         <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H7" t="n">
         <v>0</v>
@@ -1394,7 +1394,7 @@
         <v>0</v>
       </c>
       <c r="H8" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I8" t="n">
         <v>0</v>
@@ -1426,7 +1426,7 @@
         <v>0</v>
       </c>
       <c r="I9" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>